<commit_message>
updated modulator and some digital
</commit_message>
<xml_diff>
--- a/design/analog_modulator/timing.xlsx
+++ b/design/analog_modulator/timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raymond Yang\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D2405F-1F47-4CBB-BCC6-58EC78897503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6020E3A0-4EA8-4791-8F6B-C30EADCC7ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E6AD5F68-33F7-49CA-8B7F-63EB6B343C02}"/>
   </bookViews>
@@ -92,12 +92,6 @@
     <t>PULSE(0 1.8 '10u+195.3125n' 0.1n 0.1n 193.1125n 390.625n)</t>
   </si>
   <si>
-    <t>PULSE(0 1.8 10u 0.1n 0.1n 90.45625n 195.3125n)</t>
-  </si>
-  <si>
-    <t>PULSE(0 1.8 10u 0.1n 0.1n 91.45625n 195.3125n)</t>
-  </si>
-  <si>
     <t>PULSE(0 1.8 '10u+96.65625n' 0.1n 0.1n 90.45625n 195.3125n)</t>
   </si>
   <si>
@@ -108,6 +102,12 @@
   </si>
   <si>
     <t>2n</t>
+  </si>
+  <si>
+    <t>PULSE(0 1.8 '10u+2n' 0.1n 0.1n 90.45625n 195.3125n)</t>
+  </si>
+  <si>
+    <t>PULSE(0 1.8 '10u+2n' 0.1n 0.1n 91.45625n 195.3125n)</t>
   </si>
 </sst>
 </file>
@@ -247,17 +247,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -266,6 +257,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,7 +584,7 @@
   <dimension ref="C2:AB27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AF21" sqref="AF21"/>
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,28 +596,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="8" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
     </row>
     <row r="3" spans="3:28" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
@@ -692,7 +692,7 @@
       <c r="Z3" s="7">
         <v>22</v>
       </c>
-      <c r="AB3" s="13" t="s">
+      <c r="AB3" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -863,7 +863,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="1"/>
       <c r="AB13" s="6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.3">
@@ -884,7 +884,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="10"/>
+      <c r="P15" s="8"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -893,10 +893,10 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="2"/>
-      <c r="Y15" s="10"/>
+      <c r="Y15" s="8"/>
       <c r="Z15" s="3"/>
       <c r="AB15" s="6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="3:28" x14ac:dyDescent="0.3">
@@ -925,9 +925,9 @@
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
-      <c r="Z17" s="11"/>
+      <c r="Z17" s="9"/>
       <c r="AB17" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="3:28" x14ac:dyDescent="0.3">
@@ -940,7 +940,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="10"/>
+      <c r="J19" s="8"/>
       <c r="K19" s="3"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -949,20 +949,20 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="2"/>
-      <c r="S19" s="10"/>
+      <c r="S19" s="8"/>
       <c r="T19" s="3"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
-      <c r="Z19" s="11"/>
+      <c r="Z19" s="9"/>
       <c r="AB19" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -970,114 +970,114 @@
       <c r="C24" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>23</v>
+      <c r="D24" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="U24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="V24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="W24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Y24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Z24" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="12"/>
-      <c r="S26" s="12"/>
-      <c r="T26" s="12"/>
-      <c r="U26" s="12"/>
-      <c r="V26" s="12"/>
-      <c r="W26" s="12"/>
-      <c r="X26" s="12"/>
-      <c r="Y26" s="12"/>
-      <c r="Z26" s="12"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="15"/>
+      <c r="X26" s="15"/>
+      <c r="Y26" s="15"/>
+      <c r="Z26" s="15"/>
     </row>
     <row r="27" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
-      <c r="S27" s="12"/>
-      <c r="T27" s="12"/>
-      <c r="U27" s="12"/>
-      <c r="V27" s="12"/>
-      <c r="W27" s="12"/>
-      <c r="X27" s="12"/>
-      <c r="Y27" s="12"/>
-      <c r="Z27" s="12"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="15"/>
+      <c r="Y27" s="15"/>
+      <c r="Z27" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>